<commit_message>
Select numbers by size, parity, division remainder and interval
</commit_message>
<xml_diff>
--- a/TCB.xlsx
+++ b/TCB.xlsx
@@ -43,10 +43,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -57,8 +57,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -71,9 +72,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -87,30 +87,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,17 +116,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,9 +132,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,6 +166,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,13 +200,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -210,25 +210,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,7 +246,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,13 +276,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,13 +336,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,13 +348,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,25 +360,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,25 +372,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,12 +394,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -401,21 +401,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -430,6 +415,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,11 +467,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,10 +509,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -524,130 +524,130 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -974,10 +974,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2826"/>
+  <dimension ref="A1:G2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2823" sqref="Q2823"/>
+    <sheetView tabSelected="1" topLeftCell="A2799" workbookViewId="0">
+      <selection activeCell="G2827" sqref="G2827"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -65978,6 +65978,29 @@
       </c>
       <c r="G2826">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2827" spans="1:7">
+      <c r="A2827">
+        <v>1</v>
+      </c>
+      <c r="B2827">
+        <v>10</v>
+      </c>
+      <c r="C2827">
+        <v>11</v>
+      </c>
+      <c r="D2827">
+        <v>22</v>
+      </c>
+      <c r="E2827">
+        <v>26</v>
+      </c>
+      <c r="F2827">
+        <v>32</v>
+      </c>
+      <c r="G2827">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculate red01 and red06
</commit_message>
<xml_diff>
--- a/TCB.xlsx
+++ b/TCB.xlsx
@@ -44,9 +44,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -57,9 +57,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -73,21 +88,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -102,14 +110,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -124,24 +140,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,14 +156,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -172,15 +164,23 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,7 +195,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,31 +210,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,19 +228,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +276,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,61 +348,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,25 +366,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,7 +384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,6 +401,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -423,7 +456,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -443,30 +476,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -478,15 +487,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,10 +509,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -521,10 +521,10 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -533,121 +533,121 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -974,10 +974,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2827"/>
+  <dimension ref="A1:G2828"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2799" workbookViewId="0">
-      <selection activeCell="G2827" sqref="G2827"/>
+      <selection activeCell="J2828" sqref="J2828"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -66000,6 +66000,29 @@
         <v>32</v>
       </c>
       <c r="G2827">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2828" spans="1:7">
+      <c r="A2828">
+        <v>4</v>
+      </c>
+      <c r="B2828">
+        <v>10</v>
+      </c>
+      <c r="C2828">
+        <v>11</v>
+      </c>
+      <c r="D2828">
+        <v>14</v>
+      </c>
+      <c r="E2828">
+        <v>23</v>
+      </c>
+      <c r="F2828">
+        <v>32</v>
+      </c>
+      <c r="G2828">
         <v>7</v>
       </c>
     </row>

</xml_diff>